<commit_message>
update charte projet taches
</commit_message>
<xml_diff>
--- a/documentation/Planification-Taches.xlsx
+++ b/documentation/Planification-Taches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ecole\WebDynamique\web_dynamique_24632-main-LATEST\proj333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ecole\WebDynamique\web_dynamique_24632-main-LATEST\projetweb1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A7BE68-4261-4F44-81D8-76A67DF7C031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6FDB63-7BBD-4B12-A8BE-248977895352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="2565" windowWidth="26550" windowHeight="11235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Story" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="205">
   <si>
     <t>ID</t>
   </si>
@@ -676,6 +676,18 @@
   </si>
   <si>
     <t>administrer efficacement la plateforme et assurer son bon fonctionnement.</t>
+  </si>
+  <si>
+    <t>T2.0</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>Fix webdev distant server, project architecture and naming convention and enhance github version control</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1538,10 +1550,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1980,7 +1992,7 @@
         <v>194</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>194</v>
+        <v>133</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1995,288 +2007,292 @@
         <v>45881</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D17" t="s">
+        <v>204</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="H17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I17" s="11">
+        <v>45881</v>
+      </c>
+      <c r="L17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B18" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="G18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="G20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8" t="s">
-        <v>143</v>
+        <v>101</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8" t="s">
-        <v>144</v>
+        <v>103</v>
       </c>
       <c r="G24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="G25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="G26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="G27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="G28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>135</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>135</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
+    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>193</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B35" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C35" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D35" t="s">
         <v>192</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E35" t="s">
         <v>133</v>
-      </c>
-      <c r="G33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="G34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>194</v>
       </c>
       <c r="G35">
         <v>3</v>
@@ -2284,93 +2300,99 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8" t="s">
-        <v>147</v>
+        <v>111</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>163</v>
       </c>
       <c r="G36">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+    </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>58</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="G38">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B39" s="8" t="s">
+    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="G39">
-        <v>3</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>18</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="8" t="s">
-        <v>159</v>
+        <v>116</v>
       </c>
       <c r="G40">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C41" s="10"/>
-      <c r="D41" t="s">
-        <v>151</v>
+        <v>58</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="G41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H41" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="G42">
         <v>3</v>
@@ -2378,14 +2400,14 @@
     </row>
     <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8" t="s">
-        <v>66</v>
+        <v>18</v>
+      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" t="s">
+        <v>151</v>
       </c>
       <c r="G43">
         <v>3</v>
@@ -2393,14 +2415,14 @@
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>131</v>
+        <v>61</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8" t="s">
-        <v>67</v>
+        <v>146</v>
       </c>
       <c r="G44">
         <v>3</v>
@@ -2408,14 +2430,14 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>131</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G45">
         <v>3</v>
@@ -2423,14 +2445,14 @@
     </row>
     <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>131</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8" t="s">
-        <v>150</v>
+        <v>67</v>
       </c>
       <c r="G46">
         <v>3</v>
@@ -2438,14 +2460,14 @@
     </row>
     <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>131</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G47">
         <v>3</v>
@@ -2453,14 +2475,14 @@
     </row>
     <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9" t="s">
-        <v>153</v>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8" t="s">
+        <v>150</v>
       </c>
       <c r="G48">
         <v>3</v>
@@ -2468,14 +2490,14 @@
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C49" s="10"/>
-      <c r="D49" t="s">
-        <v>154</v>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="G49">
         <v>3</v>
@@ -2483,14 +2505,14 @@
     </row>
     <row r="50" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8" t="s">
-        <v>70</v>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9" t="s">
+        <v>153</v>
       </c>
       <c r="G50">
         <v>3</v>
@@ -2498,13 +2520,14 @@
     </row>
     <row r="51" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D51" s="8" t="s">
-        <v>71</v>
+      <c r="C51" s="10"/>
+      <c r="D51" t="s">
+        <v>154</v>
       </c>
       <c r="G51">
         <v>3</v>
@@ -2512,46 +2535,75 @@
     </row>
     <row r="52" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>131</v>
       </c>
+      <c r="C52" s="8"/>
       <c r="D52" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G52">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C53" s="8"/>
+        <v>131</v>
+      </c>
       <c r="D53" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>145</v>
+        <v>71</v>
       </c>
       <c r="G53">
         <v>3</v>
       </c>
-      <c r="H53" s="10" t="s">
+    </row>
+    <row r="54" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
+      <c r="H55" s="10" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L61" t="s">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L63" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C73" s="13"/>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
user guide final in pdf
</commit_message>
<xml_diff>
--- a/documentation/Planification-Taches.xlsx
+++ b/documentation/Planification-Taches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ecole\WebDynamique\web_dynamique_24632-main-LATEST\projetweb2\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ecole\WebDynamique\web_dynamique_24632-main-LATEST\projetweb1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93961684-38A2-4DE9-AEBF-590A3CAFD5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DB7154-D390-4DA9-9CAD-EA731826267A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Story" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="222">
   <si>
     <t>ID</t>
   </si>
@@ -718,6 +718,27 @@
   </si>
   <si>
     <t>3h</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>populate_database</t>
+  </si>
+  <si>
+    <t>make a script to populate site with real fake auctions</t>
+  </si>
+  <si>
+    <t>fix image upload bug</t>
+  </si>
+  <si>
+    <t>fix webdev server bug</t>
+  </si>
+  <si>
+    <t>make user guide</t>
+  </si>
+  <si>
+    <t>add screenshots and finalize user guide</t>
   </si>
 </sst>
 </file>
@@ -828,7 +849,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -874,6 +895,9 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1586,8 +1610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D35" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1595,7 +1619,7 @@
     <col min="1" max="1" width="9.6640625" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
     <col min="3" max="3" width="32.44140625" customWidth="1"/>
-    <col min="4" max="4" width="113.44140625" customWidth="1"/>
+    <col min="4" max="4" width="86.109375" customWidth="1"/>
     <col min="5" max="5" width="28.88671875" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" customWidth="1"/>
@@ -3586,7 +3610,6 @@
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="14"/>
       <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
       <c r="I59" s="14"/>
       <c r="J59" s="14"/>
       <c r="K59" s="14"/>
@@ -3596,16 +3619,23 @@
       <c r="O59" s="14"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A60" s="14"/>
+      <c r="A60" s="14" t="s">
+        <v>215</v>
+      </c>
       <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
+      <c r="C60" t="s">
+        <v>218</v>
+      </c>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
       <c r="G60" s="14"/>
       <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="14"/>
+      <c r="I60" s="16">
+        <v>45898</v>
+      </c>
+      <c r="J60" s="16">
+        <v>45898</v>
+      </c>
       <c r="K60" s="14"/>
       <c r="L60" s="14"/>
       <c r="M60" s="14"/>
@@ -3615,14 +3645,22 @@
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="14"/>
       <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
+      <c r="C61" t="s">
+        <v>219</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>217</v>
+      </c>
       <c r="E61" s="14"/>
       <c r="F61" s="14"/>
       <c r="G61" s="14"/>
       <c r="H61" s="14"/>
-      <c r="I61" s="14"/>
-      <c r="J61" s="14"/>
+      <c r="I61" s="16">
+        <v>45898</v>
+      </c>
+      <c r="J61" s="16">
+        <v>45898</v>
+      </c>
       <c r="K61" s="14"/>
       <c r="L61" s="14"/>
       <c r="M61" s="14"/>
@@ -3632,14 +3670,20 @@
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="14"/>
       <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
+      <c r="C62" s="14" t="s">
+        <v>216</v>
+      </c>
       <c r="D62" s="14"/>
       <c r="E62" s="14"/>
       <c r="F62" s="14"/>
       <c r="G62" s="14"/>
       <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
+      <c r="I62" s="16">
+        <v>45898</v>
+      </c>
+      <c r="J62" s="16">
+        <v>45898</v>
+      </c>
       <c r="K62" s="14"/>
       <c r="L62" s="14"/>
       <c r="M62" s="14"/>
@@ -3649,7 +3693,9 @@
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="14"/>
       <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
+      <c r="C63" s="14" t="s">
+        <v>220</v>
+      </c>
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
       <c r="F63" s="14"/>
@@ -3666,7 +3712,9 @@
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="14"/>
       <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
+      <c r="C64" s="14" t="s">
+        <v>221</v>
+      </c>
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
       <c r="F64" s="14"/>

</xml_diff>